<commit_message>
add more show cases
</commit_message>
<xml_diff>
--- a/WePartner/team.xlsx
+++ b/WePartner/team.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01 Project\01 Lihu\01 SF Platform\02 Sources\sf-bot-showcase-web\WePartner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41393DE-090C-4561-B645-5A9495994375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5067B4FF-A7FF-4BF9-8FB0-E6B1DCE2A714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13995" yWindow="-16485" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
@@ -244,10 +241,13 @@
     <t xml:space="preserve">lead </t>
   </si>
   <si>
-    <t>team</t>
-  </si>
-  <si>
     <t>Profile Picture</t>
+  </si>
+  <si>
+    <t>team_type</t>
+  </si>
+  <si>
+    <t>team_member_name</t>
   </si>
 </sst>
 </file>
@@ -596,14 +596,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F2" sqref="C2:F2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" style="3" customWidth="1"/>
     <col min="3" max="3" width="40.77734375" style="3" customWidth="1"/>
     <col min="4" max="4" width="129.109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="31.77734375" style="3" customWidth="1"/>
@@ -616,266 +616,266 @@
         <v>63</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:6" ht="202.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="234" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="78" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="4" t="s">
+    </row>
+    <row r="5" spans="1:6" ht="78" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="109.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="4" t="s">
+    </row>
+    <row r="7" spans="1:6" ht="156" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="171.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="218.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:6" ht="202.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="234" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="156" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:6" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="405.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="E11" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="280.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="218.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="327.60000000000002" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="140.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="265.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="124.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="D15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>